<commit_message>
Improvements for indirect solution method, Ruin & Recreate implemented
</commit_message>
<xml_diff>
--- a/V1/Dataset/OR60.xlsx
+++ b/V1/Dataset/OR60.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pylya\Desktop\PhD\PhD\github\CSPLib\V1\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A42ABFB-7E0A-43F3-B2E8-EE680B6EE006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E50D245-AE36-4C4B-9A56-8B0FCEFC187F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="22" r:id="rId1"/>
@@ -5146,18 +5146,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -5167,6 +5155,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5175,12 +5169,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5194,10 +5182,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5214,9 +5214,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5239,14 +5236,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5615,7 +5615,7 @@
       <c r="E10" s="51"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="58" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="50"/>
@@ -5638,347 +5638,347 @@
       <c r="E13" s="51"/>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="42"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="38"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="38"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="38"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="36"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="44"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="44"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="54"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="53"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="55"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="55"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="55"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="55"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="55"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="56"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="55"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="58"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="57"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="57"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="58"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="57"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="58"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="57"/>
     </row>
     <row r="27" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="56"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="55"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="55"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="56"/>
+      <c r="A28" s="54"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="55"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="55"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="56"/>
+      <c r="A29" s="54"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="55"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="60"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="60"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="33"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="60"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="33"/>
     </row>
     <row r="33" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="61" t="s">
+      <c r="A33" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="62"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="42"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="61"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="62"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="61"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="62"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="61"/>
-      <c r="B36" s="61"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="62"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="42"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="61"/>
-      <c r="B37" s="61"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="62"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="42"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="61"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="61"/>
-      <c r="E38" s="62"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="42"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="61"/>
-      <c r="B39" s="61"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="62"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="42"/>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="41"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="42"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="38"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="38"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="36"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="37"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="38"/>
+      <c r="A42" s="35"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="36"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="44"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="40"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="33" t="s">
+      <c r="A44" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="35"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="31"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="35"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="31"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="33" t="s">
+      <c r="A46" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="35"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="31"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="34"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="35"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="31"/>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="41"/>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="42"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="38"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="36" t="s">
+      <c r="A49" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="38"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="36"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="37"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="38"/>
+      <c r="A50" s="35"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="36"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="44"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="40"/>
     </row>
     <row r="52" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="32"/>
+      <c r="B52" s="59"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="60"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
       <c r="E53" s="47"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="33"/>
-      <c r="B54" s="33"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
       <c r="E54" s="47"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="59"/>
+      <c r="C55" s="59"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="60"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="32"/>
+      <c r="B56" s="59"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="60"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="26" t="s">
@@ -5987,427 +5987,439 @@
       <c r="E57" s="17"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="33" t="s">
+      <c r="A58" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="35"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="31"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="34"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="35"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="31"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="39" t="s">
+      <c r="A60" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="40"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="44"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="39"/>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="40"/>
+      <c r="A61" s="43"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="44"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="39"/>
-      <c r="B62" s="39"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="40"/>
+      <c r="A62" s="43"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="44"/>
     </row>
     <row r="63" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="41"/>
-      <c r="B63" s="41"/>
-      <c r="C63" s="41"/>
-      <c r="D63" s="41"/>
-      <c r="E63" s="42"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="38"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="36" t="s">
+      <c r="A64" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="38"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="36"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="37"/>
-      <c r="B65" s="37"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="38"/>
+      <c r="A65" s="35"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="36"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="43" t="s">
+      <c r="A66" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B66" s="43"/>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="44"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="40"/>
     </row>
     <row r="67" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="B67" s="31"/>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="32"/>
+      <c r="B67" s="59"/>
+      <c r="C67" s="59"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="60"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="29"/>
-      <c r="B68" s="29"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="30"/>
+      <c r="A68" s="45"/>
+      <c r="B68" s="45"/>
+      <c r="C68" s="45"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="46"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="36" t="s">
+      <c r="A69" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B69" s="37"/>
-      <c r="C69" s="37"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="38"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="36"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="37"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="38"/>
+      <c r="A70" s="35"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
+      <c r="E70" s="36"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="39" t="s">
+      <c r="A71" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B71" s="39"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="40"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="43"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="44"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="39"/>
-      <c r="B72" s="39"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="40"/>
+      <c r="A72" s="43"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="43"/>
+      <c r="D72" s="43"/>
+      <c r="E72" s="44"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="39"/>
-      <c r="B73" s="39"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="40"/>
+      <c r="A73" s="43"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+      <c r="E73" s="44"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="39"/>
-      <c r="B74" s="39"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="40"/>
+      <c r="A74" s="43"/>
+      <c r="B74" s="43"/>
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
+      <c r="E74" s="44"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="39"/>
-      <c r="B75" s="39"/>
-      <c r="C75" s="39"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="40"/>
+      <c r="A75" s="43"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
+      <c r="E75" s="44"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="39"/>
-      <c r="B76" s="39"/>
-      <c r="C76" s="39"/>
-      <c r="D76" s="39"/>
-      <c r="E76" s="40"/>
+      <c r="A76" s="43"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="43"/>
+      <c r="E76" s="44"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="39"/>
-      <c r="B77" s="39"/>
-      <c r="C77" s="39"/>
-      <c r="D77" s="39"/>
-      <c r="E77" s="40"/>
+      <c r="A77" s="43"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="43"/>
+      <c r="D77" s="43"/>
+      <c r="E77" s="44"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="39"/>
-      <c r="B78" s="39"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="39"/>
-      <c r="E78" s="40"/>
+      <c r="A78" s="43"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="43"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="44"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="45"/>
-      <c r="B79" s="45"/>
-      <c r="C79" s="45"/>
-      <c r="D79" s="45"/>
-      <c r="E79" s="46"/>
+      <c r="A79" s="61"/>
+      <c r="B79" s="61"/>
+      <c r="C79" s="61"/>
+      <c r="D79" s="61"/>
+      <c r="E79" s="62"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="36" t="s">
+      <c r="A80" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B80" s="37"/>
-      <c r="C80" s="37"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="38"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="36"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="37"/>
-      <c r="B81" s="37"/>
-      <c r="C81" s="37"/>
-      <c r="D81" s="37"/>
-      <c r="E81" s="38"/>
+      <c r="A81" s="35"/>
+      <c r="B81" s="35"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="35"/>
+      <c r="E81" s="36"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="39" t="s">
+      <c r="A82" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="B82" s="39"/>
-      <c r="C82" s="39"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="40"/>
+      <c r="B82" s="43"/>
+      <c r="C82" s="43"/>
+      <c r="D82" s="43"/>
+      <c r="E82" s="44"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="39"/>
-      <c r="B83" s="39"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="39"/>
-      <c r="E83" s="40"/>
+      <c r="A83" s="43"/>
+      <c r="B83" s="43"/>
+      <c r="C83" s="43"/>
+      <c r="D83" s="43"/>
+      <c r="E83" s="44"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="39"/>
-      <c r="B84" s="39"/>
-      <c r="C84" s="39"/>
-      <c r="D84" s="39"/>
-      <c r="E84" s="40"/>
+      <c r="A84" s="43"/>
+      <c r="B84" s="43"/>
+      <c r="C84" s="43"/>
+      <c r="D84" s="43"/>
+      <c r="E84" s="44"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="39"/>
-      <c r="B85" s="39"/>
-      <c r="C85" s="39"/>
-      <c r="D85" s="39"/>
-      <c r="E85" s="40"/>
+      <c r="A85" s="43"/>
+      <c r="B85" s="43"/>
+      <c r="C85" s="43"/>
+      <c r="D85" s="43"/>
+      <c r="E85" s="44"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" s="39"/>
-      <c r="B86" s="39"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="39"/>
-      <c r="E86" s="40"/>
+      <c r="A86" s="43"/>
+      <c r="B86" s="43"/>
+      <c r="C86" s="43"/>
+      <c r="D86" s="43"/>
+      <c r="E86" s="44"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="39"/>
-      <c r="B87" s="39"/>
-      <c r="C87" s="39"/>
-      <c r="D87" s="39"/>
-      <c r="E87" s="40"/>
+      <c r="A87" s="43"/>
+      <c r="B87" s="43"/>
+      <c r="C87" s="43"/>
+      <c r="D87" s="43"/>
+      <c r="E87" s="44"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="39"/>
-      <c r="B88" s="39"/>
-      <c r="C88" s="39"/>
-      <c r="D88" s="39"/>
-      <c r="E88" s="40"/>
+      <c r="A88" s="43"/>
+      <c r="B88" s="43"/>
+      <c r="C88" s="43"/>
+      <c r="D88" s="43"/>
+      <c r="E88" s="44"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" s="39"/>
-      <c r="B89" s="39"/>
-      <c r="C89" s="39"/>
-      <c r="D89" s="39"/>
-      <c r="E89" s="40"/>
+      <c r="A89" s="43"/>
+      <c r="B89" s="43"/>
+      <c r="C89" s="43"/>
+      <c r="D89" s="43"/>
+      <c r="E89" s="44"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="29"/>
-      <c r="B90" s="29"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="30"/>
+      <c r="A90" s="45"/>
+      <c r="B90" s="45"/>
+      <c r="C90" s="45"/>
+      <c r="D90" s="45"/>
+      <c r="E90" s="46"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="36" t="s">
+      <c r="A91" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B91" s="37"/>
-      <c r="C91" s="37"/>
-      <c r="D91" s="37"/>
-      <c r="E91" s="38"/>
+      <c r="B91" s="35"/>
+      <c r="C91" s="35"/>
+      <c r="D91" s="35"/>
+      <c r="E91" s="36"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="37"/>
-      <c r="B92" s="37"/>
-      <c r="C92" s="37"/>
-      <c r="D92" s="37"/>
-      <c r="E92" s="38"/>
+      <c r="A92" s="35"/>
+      <c r="B92" s="35"/>
+      <c r="C92" s="35"/>
+      <c r="D92" s="35"/>
+      <c r="E92" s="36"/>
     </row>
     <row r="93" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="39" t="s">
+      <c r="A93" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="B93" s="39"/>
-      <c r="C93" s="39"/>
-      <c r="D93" s="39"/>
-      <c r="E93" s="40"/>
+      <c r="B93" s="43"/>
+      <c r="C93" s="43"/>
+      <c r="D93" s="43"/>
+      <c r="E93" s="44"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" s="39"/>
-      <c r="B94" s="39"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="40"/>
+      <c r="A94" s="43"/>
+      <c r="B94" s="43"/>
+      <c r="C94" s="43"/>
+      <c r="D94" s="43"/>
+      <c r="E94" s="44"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" s="39"/>
-      <c r="B95" s="39"/>
-      <c r="C95" s="39"/>
-      <c r="D95" s="39"/>
-      <c r="E95" s="40"/>
+      <c r="A95" s="43"/>
+      <c r="B95" s="43"/>
+      <c r="C95" s="43"/>
+      <c r="D95" s="43"/>
+      <c r="E95" s="44"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" s="39"/>
-      <c r="B96" s="39"/>
-      <c r="C96" s="39"/>
-      <c r="D96" s="39"/>
-      <c r="E96" s="40"/>
+      <c r="A96" s="43"/>
+      <c r="B96" s="43"/>
+      <c r="C96" s="43"/>
+      <c r="D96" s="43"/>
+      <c r="E96" s="44"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" s="39"/>
-      <c r="B97" s="39"/>
-      <c r="C97" s="39"/>
-      <c r="D97" s="39"/>
-      <c r="E97" s="40"/>
+      <c r="A97" s="43"/>
+      <c r="B97" s="43"/>
+      <c r="C97" s="43"/>
+      <c r="D97" s="43"/>
+      <c r="E97" s="44"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" s="39"/>
-      <c r="B98" s="39"/>
-      <c r="C98" s="39"/>
-      <c r="D98" s="39"/>
-      <c r="E98" s="40"/>
+      <c r="A98" s="43"/>
+      <c r="B98" s="43"/>
+      <c r="C98" s="43"/>
+      <c r="D98" s="43"/>
+      <c r="E98" s="44"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" s="39"/>
-      <c r="B99" s="39"/>
-      <c r="C99" s="39"/>
-      <c r="D99" s="39"/>
-      <c r="E99" s="40"/>
+      <c r="A99" s="43"/>
+      <c r="B99" s="43"/>
+      <c r="C99" s="43"/>
+      <c r="D99" s="43"/>
+      <c r="E99" s="44"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" s="39"/>
-      <c r="B100" s="39"/>
-      <c r="C100" s="39"/>
-      <c r="D100" s="39"/>
-      <c r="E100" s="40"/>
+      <c r="A100" s="43"/>
+      <c r="B100" s="43"/>
+      <c r="C100" s="43"/>
+      <c r="D100" s="43"/>
+      <c r="E100" s="44"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101" s="29"/>
-      <c r="B101" s="29"/>
-      <c r="C101" s="29"/>
-      <c r="D101" s="29"/>
-      <c r="E101" s="30"/>
+      <c r="A101" s="45"/>
+      <c r="B101" s="45"/>
+      <c r="C101" s="45"/>
+      <c r="D101" s="45"/>
+      <c r="E101" s="46"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" s="36" t="s">
+      <c r="A102" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B102" s="37"/>
-      <c r="C102" s="37"/>
-      <c r="D102" s="37"/>
-      <c r="E102" s="38"/>
+      <c r="B102" s="35"/>
+      <c r="C102" s="35"/>
+      <c r="D102" s="35"/>
+      <c r="E102" s="36"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" s="37"/>
-      <c r="B103" s="37"/>
-      <c r="C103" s="37"/>
-      <c r="D103" s="37"/>
-      <c r="E103" s="38"/>
+      <c r="A103" s="35"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="36"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" s="39" t="s">
+      <c r="A104" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B104" s="39"/>
-      <c r="C104" s="39"/>
-      <c r="D104" s="39"/>
-      <c r="E104" s="40"/>
+      <c r="B104" s="43"/>
+      <c r="C104" s="43"/>
+      <c r="D104" s="43"/>
+      <c r="E104" s="44"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" s="39"/>
-      <c r="B105" s="39"/>
-      <c r="C105" s="39"/>
-      <c r="D105" s="39"/>
-      <c r="E105" s="40"/>
+      <c r="A105" s="43"/>
+      <c r="B105" s="43"/>
+      <c r="C105" s="43"/>
+      <c r="D105" s="43"/>
+      <c r="E105" s="44"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" s="39"/>
-      <c r="B106" s="39"/>
-      <c r="C106" s="39"/>
-      <c r="D106" s="39"/>
-      <c r="E106" s="40"/>
+      <c r="A106" s="43"/>
+      <c r="B106" s="43"/>
+      <c r="C106" s="43"/>
+      <c r="D106" s="43"/>
+      <c r="E106" s="44"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" s="39"/>
-      <c r="B107" s="39"/>
-      <c r="C107" s="39"/>
-      <c r="D107" s="39"/>
-      <c r="E107" s="40"/>
+      <c r="A107" s="43"/>
+      <c r="B107" s="43"/>
+      <c r="C107" s="43"/>
+      <c r="D107" s="43"/>
+      <c r="E107" s="44"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" s="39"/>
-      <c r="B108" s="39"/>
-      <c r="C108" s="39"/>
-      <c r="D108" s="39"/>
-      <c r="E108" s="40"/>
+      <c r="A108" s="43"/>
+      <c r="B108" s="43"/>
+      <c r="C108" s="43"/>
+      <c r="D108" s="43"/>
+      <c r="E108" s="44"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109" s="39"/>
-      <c r="B109" s="39"/>
-      <c r="C109" s="39"/>
-      <c r="D109" s="39"/>
-      <c r="E109" s="40"/>
+      <c r="A109" s="43"/>
+      <c r="B109" s="43"/>
+      <c r="C109" s="43"/>
+      <c r="D109" s="43"/>
+      <c r="E109" s="44"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A110" s="39"/>
-      <c r="B110" s="39"/>
-      <c r="C110" s="39"/>
-      <c r="D110" s="39"/>
-      <c r="E110" s="40"/>
+      <c r="A110" s="43"/>
+      <c r="B110" s="43"/>
+      <c r="C110" s="43"/>
+      <c r="D110" s="43"/>
+      <c r="E110" s="44"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A111" s="39"/>
-      <c r="B111" s="39"/>
-      <c r="C111" s="39"/>
-      <c r="D111" s="39"/>
-      <c r="E111" s="40"/>
+      <c r="A111" s="43"/>
+      <c r="B111" s="43"/>
+      <c r="C111" s="43"/>
+      <c r="D111" s="43"/>
+      <c r="E111" s="44"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="29"/>
-      <c r="B112" s="29"/>
-      <c r="C112" s="29"/>
-      <c r="D112" s="29"/>
-      <c r="E112" s="30"/>
+      <c r="A112" s="45"/>
+      <c r="B112" s="45"/>
+      <c r="C112" s="45"/>
+      <c r="D112" s="45"/>
+      <c r="E112" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A44:E45"/>
-    <mergeCell ref="A46:E47"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A41:E42"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:E39"/>
+    <mergeCell ref="A112:E112"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="A58:E59"/>
+    <mergeCell ref="A91:E92"/>
+    <mergeCell ref="A93:E100"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="A69:E70"/>
+    <mergeCell ref="A60:E62"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A64:E65"/>
+    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A71:E78"/>
+    <mergeCell ref="A102:E103"/>
+    <mergeCell ref="A104:E111"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E50"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A79:E79"/>
     <mergeCell ref="A80:E81"/>
     <mergeCell ref="A82:E89"/>
     <mergeCell ref="A90:E90"/>
@@ -6424,27 +6436,15 @@
     <mergeCell ref="A20:E21"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="A27:E29"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A49:E50"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="A112:E112"/>
-    <mergeCell ref="A56:E56"/>
-    <mergeCell ref="A58:E59"/>
-    <mergeCell ref="A91:E92"/>
-    <mergeCell ref="A93:E100"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="A69:E70"/>
-    <mergeCell ref="A60:E62"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A64:E65"/>
-    <mergeCell ref="A66:E66"/>
-    <mergeCell ref="A67:E67"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A71:E78"/>
-    <mergeCell ref="A102:E103"/>
-    <mergeCell ref="A104:E111"/>
+    <mergeCell ref="A44:E45"/>
+    <mergeCell ref="A46:E47"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A41:E42"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A33:E39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8063,8 +8063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B4773B-09CB-4AE1-B7A2-EA1A4F4D3191}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8117,7 +8117,7 @@
         <v>54</v>
       </c>
       <c r="E3" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -8131,7 +8131,7 @@
         <v>55</v>
       </c>
       <c r="E4" s="24">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -8145,7 +8145,7 @@
         <v>56</v>
       </c>
       <c r="E5" s="24">
-        <v>4</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -8153,7 +8153,7 @@
         <v>57</v>
       </c>
       <c r="E6" s="24">
-        <v>5</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -8161,7 +8161,7 @@
         <v>58</v>
       </c>
       <c r="E7" s="24">
-        <v>6</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -8169,7 +8169,7 @@
         <v>59</v>
       </c>
       <c r="E8" s="24">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -8177,7 +8177,7 @@
         <v>95</v>
       </c>
       <c r="E9" s="24">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -8185,7 +8185,7 @@
         <v>111</v>
       </c>
       <c r="E10" s="24">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -8193,7 +8193,7 @@
         <v>94</v>
       </c>
       <c r="E11" s="24">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -8201,7 +8201,7 @@
         <v>93</v>
       </c>
       <c r="E12" s="24">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -8209,7 +8209,7 @@
         <v>60</v>
       </c>
       <c r="E13" s="24">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -8217,7 +8217,7 @@
         <v>61</v>
       </c>
       <c r="E14" s="24">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -8225,7 +8225,7 @@
         <v>62</v>
       </c>
       <c r="E15" s="24">
-        <v>14</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -8233,7 +8233,7 @@
         <v>63</v>
       </c>
       <c r="E16" s="24">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.3">
@@ -8241,7 +8241,7 @@
         <v>84</v>
       </c>
       <c r="E17" s="24">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.3">
@@ -8249,7 +8249,7 @@
         <v>92</v>
       </c>
       <c r="E18" s="24">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.3">
@@ -8257,7 +8257,7 @@
         <v>98</v>
       </c>
       <c r="E19" s="24">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.3">
@@ -8265,7 +8265,7 @@
         <v>99</v>
       </c>
       <c r="E20" s="24">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.3">
@@ -8273,7 +8273,7 @@
         <v>100</v>
       </c>
       <c r="E21" s="24">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.3">
@@ -8281,7 +8281,7 @@
         <v>104</v>
       </c>
       <c r="E22" s="24">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.3">
@@ -8289,7 +8289,7 @@
         <v>105</v>
       </c>
       <c r="E23" s="24">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.3">
@@ -8297,7 +8297,7 @@
         <v>102</v>
       </c>
       <c r="E24" s="24">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.3">
@@ -8305,7 +8305,7 @@
         <v>103</v>
       </c>
       <c r="E25" s="24">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.3">
@@ -8313,7 +8313,7 @@
         <v>106</v>
       </c>
       <c r="E26" s="24">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.3">
@@ -8321,7 +8321,7 @@
         <v>107</v>
       </c>
       <c r="E27" s="24">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.3">
@@ -8329,7 +8329,7 @@
         <v>108</v>
       </c>
       <c r="E28" s="24">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.3">
@@ -8337,7 +8337,7 @@
         <v>109</v>
       </c>
       <c r="E29" s="24">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>